<commit_message>
added changes to scrum artifacts
</commit_message>
<xml_diff>
--- a/Planning and Design/Scrum Artifacts.xlsx
+++ b/Planning and Design/Scrum Artifacts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donal\source\repos\CST-247-Milestone-CLC\Planning and Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryke\source\repos\CST-247-Milestone-CLC\Planning and Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB86CD41-56B4-4A59-865F-D923BD99B94E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8000E98-E40D-4FC2-A911-7D8F0C4573E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30420" yWindow="2145" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burn Chart" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="62">
   <si>
     <t>Sprint Goals</t>
   </si>
@@ -1484,88 +1484,88 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>106</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>104</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>104</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>96</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>92</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>89</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>89</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>86</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>78</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>67</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>59</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>51</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>49</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>49</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>49</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>49</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>49</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>49</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>49</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>49</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>49</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>49</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>49</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>49</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>44</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>0</c:v>
@@ -2465,7 +2465,7 @@
   </sheetPr>
   <dimension ref="A1:Z940"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -2573,7 +2573,7 @@
       </c>
       <c r="H3" s="11">
         <f>IF(G3=0,"",C9 - G3)</f>
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -2617,7 +2617,7 @@
       </c>
       <c r="H4" s="11">
         <f t="shared" ref="H4:H37" si="0">IF(G4="","",H3 - G4)</f>
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -2660,7 +2660,7 @@
       </c>
       <c r="H5" s="11">
         <f t="shared" si="0"/>
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="H6" s="11">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -2731,11 +2731,11 @@
       </c>
       <c r="B7" s="7">
         <f>'Sprint 5'!D$9</f>
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C7" s="8">
         <f>'Sprint 5'!D$10</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="28"/>
@@ -2748,7 +2748,7 @@
       </c>
       <c r="H7" s="11">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="H8" s="11">
         <f t="shared" si="0"/>
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -2812,7 +2812,7 @@
       </c>
       <c r="C9" s="13">
         <f>SUM(B3:B7)</f>
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="29"/>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="H9" s="11">
         <f t="shared" si="0"/>
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -2862,7 +2862,7 @@
       </c>
       <c r="H10" s="11">
         <f>IF(G10="","",H9 - G10)</f>
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -2897,7 +2897,7 @@
       </c>
       <c r="H11" s="11">
         <f t="shared" si="0"/>
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -2933,7 +2933,7 @@
       </c>
       <c r="H12" s="11">
         <f t="shared" si="0"/>
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -2969,7 +2969,7 @@
       </c>
       <c r="H13" s="11">
         <f t="shared" si="0"/>
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="H14" s="11">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="H15" s="11">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -3077,7 +3077,7 @@
       </c>
       <c r="H16" s="11">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -3115,7 +3115,7 @@
       </c>
       <c r="H17" s="11">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -3150,7 +3150,7 @@
       </c>
       <c r="H18" s="11">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -3185,7 +3185,7 @@
       </c>
       <c r="H19" s="11">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -3220,7 +3220,7 @@
       </c>
       <c r="H20" s="11">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -3255,7 +3255,7 @@
       </c>
       <c r="H21" s="11">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -3290,7 +3290,7 @@
       </c>
       <c r="H22" s="11">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -3325,7 +3325,7 @@
       </c>
       <c r="H23" s="11">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -3362,7 +3362,7 @@
       </c>
       <c r="H24" s="11">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -3397,7 +3397,7 @@
       </c>
       <c r="H25" s="11">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -3432,7 +3432,7 @@
       </c>
       <c r="H26" s="11">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -3467,7 +3467,7 @@
       </c>
       <c r="H27" s="11">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -3502,7 +3502,7 @@
       </c>
       <c r="H28" s="11">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -3538,7 +3538,7 @@
       </c>
       <c r="H29" s="11">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -3574,7 +3574,7 @@
       </c>
       <c r="H30" s="11">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -59155,8 +59155,8 @@
   </sheetPr>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -59201,19 +59201,19 @@
         <v>56</v>
       </c>
       <c r="B2" s="20">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C2" s="20">
         <f>SUMIF(I2:I50, A2, J2:J50)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D2" s="20">
         <f t="shared" ref="D2:D3" si="0">B2-C2</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E2" s="21">
         <f t="shared" ref="E2:E3" si="1">C2/B2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="30">
@@ -59289,7 +59289,7 @@
       </c>
       <c r="D9" s="24">
         <f>SUM(B2:B4)</f>
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G9" s="34">
         <v>2</v>
@@ -59304,7 +59304,7 @@
       </c>
       <c r="D10" s="24">
         <f>SUM(D2:D4)</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G10" s="28"/>
       <c r="H10" s="9"/>
@@ -59433,9 +59433,15 @@
       <c r="G30" s="30">
         <v>5</v>
       </c>
-      <c r="H30" s="9"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="11"/>
+      <c r="H30" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J30" s="11">
+        <v>4</v>
+      </c>
     </row>
     <row r="31" spans="7:10" ht="15.75" customHeight="1">
       <c r="G31" s="28"/>
@@ -59477,9 +59483,15 @@
       <c r="G37" s="34">
         <v>6</v>
       </c>
-      <c r="H37" s="9"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="11"/>
+      <c r="H37" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J37" s="11">
+        <v>4</v>
+      </c>
     </row>
     <row r="38" spans="7:10" ht="15">
       <c r="G38" s="28"/>
@@ -59521,9 +59533,15 @@
       <c r="G44" s="35">
         <v>7</v>
       </c>
-      <c r="H44" s="9"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="11"/>
+      <c r="H44" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J44" s="11">
+        <v>2</v>
+      </c>
     </row>
     <row r="45" spans="7:10" ht="15">
       <c r="G45" s="28"/>

</xml_diff>